<commit_message>
Dumbwaiter teleport and Intro scene
Made the ladder trigger the dumbwaiter floor as a valid teleport target

Added the Intro scene (text and flow only, sound to come)
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caras\UnityProjects\TheNewRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C03DCCD-B3D0-4AB0-9A71-DB12CF468FCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A195D37-7F10-43D3-BA51-C74E1F2098A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2445" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>Done</t>
   </si>
@@ -42,15 +42,6 @@
     <t>Opening</t>
   </si>
   <si>
-    <t>Title Page</t>
-  </si>
-  <si>
-    <t>Buttons for Sitting/Standing</t>
-  </si>
-  <si>
-    <t>Button for Start</t>
-  </si>
-  <si>
     <t>Intro</t>
   </si>
   <si>
@@ -63,12 +54,6 @@
     <t>Bang of door</t>
   </si>
   <si>
-    <t>VO of owner (Look down, intructions)</t>
-  </si>
-  <si>
-    <t>Scuffle from behind door, owner dragged away</t>
-  </si>
-  <si>
     <t>Main</t>
   </si>
   <si>
@@ -108,9 +93,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Started</t>
-  </si>
-  <si>
     <t>Puzzles</t>
   </si>
   <si>
@@ -144,9 +126,6 @@
     <t>Inventory viewing</t>
   </si>
   <si>
-    <t>Nearly done - positioning is off</t>
-  </si>
-  <si>
     <t>Make ladder necessary to teleport into dumbwaiter</t>
   </si>
   <si>
@@ -174,10 +153,43 @@
     <t>Keg colour clue in drawer</t>
   </si>
   <si>
-    <t>Start ambient music</t>
-  </si>
-  <si>
-    <t>Found</t>
+    <t>Abandoned - not practical with this layout</t>
+  </si>
+  <si>
+    <t>Nearly done - return positioning is off</t>
+  </si>
+  <si>
+    <t>Exit Function</t>
+  </si>
+  <si>
+    <t>Intro Scene</t>
+  </si>
+  <si>
+    <t>Menu Scene</t>
+  </si>
+  <si>
+    <t>Narration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VO of owner </t>
+  </si>
+  <si>
+    <t>Door handle on inside of top door (non functional)</t>
+  </si>
+  <si>
+    <t>Ambient music</t>
+  </si>
+  <si>
+    <t>Win music</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Animation  of middle cask opening</t>
+  </si>
+  <si>
+    <t>Credits scene</t>
   </si>
 </sst>
 </file>
@@ -495,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,13 +524,13 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,10 +541,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,7 +552,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -548,64 +560,59 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
         <v>0</v>
@@ -613,7 +620,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
@@ -621,7 +628,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>0</v>
@@ -629,7 +636,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -637,7 +644,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -645,7 +652,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -653,7 +660,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -661,18 +668,15 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>19</v>
-      </c>
       <c r="C18" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -680,15 +684,15 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" t="s">
-        <v>0</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
@@ -696,42 +700,42 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>28</v>
-      </c>
       <c r="C23" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="D23" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -739,12 +743,15 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>40</v>
+        <v>24</v>
+      </c>
+      <c r="D26" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
@@ -752,23 +759,23 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>33</v>
-      </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
@@ -776,40 +783,89 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>28</v>
+      </c>
+      <c r="D31" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>1</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>38</v>
       </c>
-      <c r="D31" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D34" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>40</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added end sequence (most of it)
Added animation for barrel lid
Added panel that will fade to black
Added hidden door
Added message to stay tuned for Chapter 2
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caras\UnityProjects\TheNewRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A195D37-7F10-43D3-BA51-C74E1F2098A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0121FBDE-EB38-405D-B59E-65A4E412B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2445" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
   <si>
     <t>Done</t>
   </si>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +554,9 @@
       <c r="C3" t="s">
         <v>44</v>
       </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -866,6 +869,9 @@
       </c>
       <c r="C40" t="s">
         <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Scene transitions and added narration
Finally good enough to attempt to build!! May tweak voice overs, but game is essentially finished!
</commit_message>
<xml_diff>
--- a/TODO.xlsx
+++ b/TODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\caras\UnityProjects\TheNewRecipe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0121FBDE-EB38-405D-B59E-65A4E412B9EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E099C22C-A1B2-4EE1-8341-CF5B44ED71D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2445" yWindow="1785" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="61">
   <si>
     <t>Done</t>
   </si>
@@ -190,14 +190,40 @@
   </si>
   <si>
     <t>Credits scene</t>
+  </si>
+  <si>
+    <t>Trigger Stay Tuned panel</t>
+  </si>
+  <si>
+    <t>Transitions</t>
+  </si>
+  <si>
+    <t>Menu to Instructions</t>
+  </si>
+  <si>
+    <t>Menu to Intro</t>
+  </si>
+  <si>
+    <t>Intro to Chapter 1</t>
+  </si>
+  <si>
+    <t>Done!!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -225,8 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,16 +547,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
@@ -579,6 +606,9 @@
       <c r="C5" t="s">
         <v>47</v>
       </c>
+      <c r="D5" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
@@ -587,6 +617,9 @@
       <c r="C6" t="s">
         <v>8</v>
       </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -595,6 +628,9 @@
       <c r="C7" t="s">
         <v>48</v>
       </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
@@ -607,39 +643,48 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B13" t="s">
         <v>10</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C13" t="s">
         <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
@@ -647,7 +692,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
         <v>0</v>
@@ -655,7 +700,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
@@ -663,7 +708,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D16" t="s">
         <v>0</v>
@@ -671,7 +716,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
         <v>0</v>
@@ -679,7 +724,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
         <v>0</v>
@@ -687,15 +732,15 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>49</v>
+        <v>26</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
         <v>0</v>
@@ -703,7 +748,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D21" t="s">
         <v>0</v>
@@ -711,34 +756,34 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="D22" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D23" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>22</v>
-      </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D25" t="s">
         <v>0</v>
@@ -746,23 +791,26 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D27" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>22</v>
+      </c>
       <c r="C28" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D28" t="s">
         <v>0</v>
@@ -770,7 +818,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
         <v>0</v>
@@ -778,37 +826,31 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>27</v>
-      </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>1</v>
-      </c>
       <c r="C33" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
         <v>0</v>
@@ -816,65 +858,110 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D34" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
+        <v>37</v>
+      </c>
+      <c r="D35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
         <v>40</v>
       </c>
-      <c r="D35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" t="s">
+      <c r="D38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>41</v>
       </c>
-      <c r="D36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="D39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>52</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>7</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>51</v>
       </c>
-      <c r="D38" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="D41" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
         <v>10</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="D42" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D43" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C44" t="s">
         <v>54</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D44" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>